<commit_message>
Update barbarian unit test spreadsheet
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/BlackBox_Barbarian.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/BlackBox_Barbarian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AFB2E9-5F61-40EE-BD3C-599232FC881D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DB9A46-42D8-472C-9C18-FF3C391252D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Test Case</t>
   </si>
@@ -52,13 +52,40 @@
   </si>
   <si>
     <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Level 6</t>
+  </si>
+  <si>
+    <t>Level 7</t>
+  </si>
+  <si>
+    <t>Level 8</t>
+  </si>
+  <si>
+    <t>Level 9</t>
+  </si>
+  <si>
+    <t>Level 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +105,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +489,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
@@ -464,6 +497,159 @@
       </c>
       <c r="E3" s="4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -474,6 +660,7 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>